<commit_message>
did my user story specs on commands I've completed
meh
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/User Story Specs.xlsx
+++ b/Homework Assignments/a15/User Story Specs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Desktop\skewl\2018 Fall\Software Engineering\a15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A302A070-2A21-452E-8DED-8C0336295896}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{095058D2-CBB2-42D5-A2A8-C81862E817C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>User Story</t>
   </si>
@@ -48,27 +48,6 @@
     <t>Team Members:</t>
   </si>
   <si>
-    <t>I, Joe, as a student of Texas State University would like to be able to find open bike racks on campus before I come to campus so that I don't waste my time looking.</t>
-  </si>
-  <si>
-    <t>Display a list of open bike racks</t>
-  </si>
-  <si>
-    <t>Search function for open bike racks near my destination</t>
-  </si>
-  <si>
-    <t>Ability to reserve a location on a bike rack.</t>
-  </si>
-  <si>
-    <t>Whether the bike racks are lighted at night</t>
-  </si>
-  <si>
-    <t>Ability to report the number of open slots on a bike rack.</t>
-  </si>
-  <si>
-    <t>Ability to report the typical times a bike rack has at least one open slot.</t>
-  </si>
-  <si>
     <t>User Stories &amp; Functional Requirements for GetRichTwitch</t>
   </si>
   <si>
@@ -88,6 +67,39 @@
   </si>
   <si>
     <t>example:</t>
+  </si>
+  <si>
+    <t>I, |slartibartfast|, am a Twitch user that wants to have fun in Twitch chat. I type "!slap" and then the name of another user in chat to slap them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bot slaps the wanted user, typing @[username] You Have Been Slapped! </t>
+  </si>
+  <si>
+    <t>Searches the running list of usernames that have posted in the chat, tells slaper whether slapee is in chat.</t>
+  </si>
+  <si>
+    <t>keep a tally of who has been slapped the most</t>
+  </si>
+  <si>
+    <t>An actual hand coming out of the computer to slap someone, because it is all digital and fake internet points.</t>
+  </si>
+  <si>
+    <t>permissions, only certain users can slap</t>
+  </si>
+  <si>
+    <t>I, XxMaestroChefxX is a Twitch user that wants to see their status. They type "!stats" in chat.</t>
+  </si>
+  <si>
+    <t>The bot responds with information on their status including name, if they are a mod, and badges.</t>
+  </si>
+  <si>
+    <t>also includes information on their points, coins, and other chat games information.</t>
+  </si>
+  <si>
+    <t>stores information in a file for data mining/management for use of account using bot.</t>
+  </si>
+  <si>
+    <t>Personal information will not be stored.</t>
   </si>
 </sst>
 </file>
@@ -162,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -180,6 +192,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -464,7 +479,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,7 +493,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3"/>
@@ -487,19 +502,19 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -530,47 +545,61 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+    <row r="10" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>

</xml_diff>

<commit_message>
Added my user story to Asg15
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/User Story Specs.xlsx
+++ b/Homework Assignments/a15/User Story Specs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{095058D2-CBB2-42D5-A2A8-C81862E817C2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>User Story</t>
   </si>
@@ -100,12 +99,42 @@
   </si>
   <si>
     <t>Personal information will not be stored.</t>
+  </si>
+  <si>
+    <t>I, MasterTwitchUser, is a Twitch user that has just subscribed to the channel.</t>
+  </si>
+  <si>
+    <t>Logs name and can store the subscriptions in a data file for mining purposes.</t>
+  </si>
+  <si>
+    <t>Won't print out a message to the views showing the user subscribed becauser that is already built into Twitch.</t>
+  </si>
+  <si>
+    <t>The bot recognized the subscription of a user.</t>
+  </si>
+  <si>
+    <t>Should loga a message out of the chats view.</t>
+  </si>
+  <si>
+    <t>I, TheGreatGabby01, is a Twitch user that wants to gamble some of their coins for potentailly more coins. They type "!gamble xxx" in chat. xxx = heads/tails</t>
+  </si>
+  <si>
+    <t>The bot deducts coins from the user and then flips a coin to see if they won or not.</t>
+  </si>
+  <si>
+    <t>Access to the the data files where we keep all the users' coins and points.</t>
+  </si>
+  <si>
+    <t>A flashy message that shows the user gambling in chat for others to see.</t>
+  </si>
+  <si>
+    <t>A graphical image that moves to show that the user won or not.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,14 +216,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,11 +504,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,18 +547,18 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -553,7 +582,7 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -573,7 +602,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
@@ -582,7 +611,7 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -601,19 +630,45 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
+    <row r="11" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>

</xml_diff>

<commit_message>
correct formatting according to assignment sheet
I hate this shit
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/User Story Specs.xlsx
+++ b/Homework Assignments/a15/User Story Specs.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E25C2C8D-92DC-4089-9BB1-46B533BC2C0F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
   <si>
     <t>User Story</t>
   </si>
@@ -65,30 +66,12 @@
     <t>Joel</t>
   </si>
   <si>
-    <t>example:</t>
-  </si>
-  <si>
-    <t>I, |slartibartfast|, am a Twitch user that wants to have fun in Twitch chat. I type "!slap" and then the name of another user in chat to slap them.</t>
-  </si>
-  <si>
     <t xml:space="preserve">The bot slaps the wanted user, typing @[username] You Have Been Slapped! </t>
   </si>
   <si>
-    <t>Searches the running list of usernames that have posted in the chat, tells slaper whether slapee is in chat.</t>
-  </si>
-  <si>
-    <t>keep a tally of who has been slapped the most</t>
-  </si>
-  <si>
     <t>An actual hand coming out of the computer to slap someone, because it is all digital and fake internet points.</t>
   </si>
   <si>
-    <t>permissions, only certain users can slap</t>
-  </si>
-  <si>
-    <t>I, XxMaestroChefxX is a Twitch user that wants to see their status. They type "!stats" in chat.</t>
-  </si>
-  <si>
     <t>The bot responds with information on their status including name, if they are a mod, and badges.</t>
   </si>
   <si>
@@ -129,13 +112,49 @@
   </si>
   <si>
     <t>A graphical image that moves to show that the user won or not.</t>
+  </si>
+  <si>
+    <t>The Bot receives the message</t>
+  </si>
+  <si>
+    <t>Searches the running list of usernames that have posted in the chat.</t>
+  </si>
+  <si>
+    <t>backslap, those are just rude.</t>
+  </si>
+  <si>
+    <t>I, Levi, am a Twitch user called |slartibartfast|, I want to have fun in Twitch chat. I type "!slap" and then the name of another user in chat to slap them.</t>
+  </si>
+  <si>
+    <t>I,Levi, am a Twitch user called  XxMaestroChefxX, I want to see their status. They type "!stats" in chat.</t>
+  </si>
+  <si>
+    <t>No separate mod functionality.</t>
+  </si>
+  <si>
+    <t>Nifty formatting.</t>
+  </si>
+  <si>
+    <t>Tells the user the information that is stored for the channel to use.</t>
+  </si>
+  <si>
+    <t>Keep a tally of who has been slapped the most.</t>
+  </si>
+  <si>
+    <t>Tells slaper whether slapee is in chat.</t>
+  </si>
+  <si>
+    <t>The Bot receives the message.</t>
+  </si>
+  <si>
+    <t>Permissions, only certain users can slap.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,14 +178,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -176,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -199,11 +210,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -211,9 +240,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -224,6 +250,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -504,11 +542,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,18 +585,18 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -572,117 +610,127 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="D10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4" t="s">
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10"/>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="E12" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+    <row r="13" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
@@ -754,11 +802,28 @@
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated my user story
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/User Story Specs.xlsx
+++ b/Homework Assignments/a15/User Story Specs.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E25C2C8D-92DC-4089-9BB1-46B533BC2C0F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
   <si>
     <t>User Story</t>
   </si>
@@ -84,24 +83,9 @@
     <t>Personal information will not be stored.</t>
   </si>
   <si>
-    <t>I, MasterTwitchUser, is a Twitch user that has just subscribed to the channel.</t>
-  </si>
-  <si>
-    <t>Logs name and can store the subscriptions in a data file for mining purposes.</t>
-  </si>
-  <si>
-    <t>Won't print out a message to the views showing the user subscribed becauser that is already built into Twitch.</t>
-  </si>
-  <si>
     <t>The bot recognized the subscription of a user.</t>
   </si>
   <si>
-    <t>Should loga a message out of the chats view.</t>
-  </si>
-  <si>
-    <t>I, TheGreatGabby01, is a Twitch user that wants to gamble some of their coins for potentailly more coins. They type "!gamble xxx" in chat. xxx = heads/tails</t>
-  </si>
-  <si>
     <t>The bot deducts coins from the user and then flips a coin to see if they won or not.</t>
   </si>
   <si>
@@ -148,12 +132,51 @@
   </si>
   <si>
     <t>Permissions, only certain users can slap.</t>
+  </si>
+  <si>
+    <t>I, Joel, am a Twitch user called MasterTwitchUser that has just subscribed to the channel.</t>
+  </si>
+  <si>
+    <t>Bot doesn't recognize a user trying to imitate a sub using a chat message.</t>
+  </si>
+  <si>
+    <t>Should log a message out of the chats view.</t>
+  </si>
+  <si>
+    <t>Should have the ablity to work on a Twitch Prime sub and other sub types.</t>
+  </si>
+  <si>
+    <t>Logs name and can stores the subscriptions in a data file for mining purposes.</t>
+  </si>
+  <si>
+    <t>A bot message congratulating the user for subscribing.</t>
+  </si>
+  <si>
+    <t>Won't print out a message to the views showing the user subscribed because that is already built into Twitch.</t>
+  </si>
+  <si>
+    <t>Give the user coins of points for subscribing.</t>
+  </si>
+  <si>
+    <t>I, Joel, am a Twitch user TheGreatGabby01 who wants to gamble some of their coins for potentailly more coins. I can type "!gamble xxx" in chat. xxx = heads/tails</t>
+  </si>
+  <si>
+    <t>Stop the user from gambling if they don't have enough coins.</t>
+  </si>
+  <si>
+    <t>The ability to check, add, and deduct points from the user.</t>
+  </si>
+  <si>
+    <t>Other people placing bets on that person's bet.</t>
+  </si>
+  <si>
+    <t>Won't have any monetary value because I believe that's illegal.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -245,6 +268,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -255,9 +281,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -542,11 +565,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,18 +608,18 @@
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="3" t="s">
         <v>1</v>
       </c>
@@ -611,17 +634,17 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>14</v>
@@ -629,39 +652,39 @@
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>33</v>
+      <c r="A9" s="9" t="s">
+        <v>28</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
@@ -669,7 +692,7 @@
         <v>17</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>18</v>
@@ -678,59 +701,71 @@
     </row>
     <row r="11" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="4"/>
+    </row>
+    <row r="13" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="4"/>
+    </row>
+    <row r="14" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+      <c r="B14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="4"/>
-    </row>
-    <row r="14" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>

</xml_diff>

<commit_message>
i accidentally added a border earlier
deleted border
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/User Story Specs.xlsx
+++ b/Homework Assignments/a15/User Story Specs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Levi\Documents\GitHub\GetRichTwitch\Homework Assignments\a15\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B469D4FE-8121-4829-80AB-DBD3EB9BFC16}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -176,7 +177,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,7 +211,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -233,29 +234,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -280,11 +263,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -565,11 +545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +650,7 @@
       <c r="A9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="10" t="s">
         <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -684,7 +664,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="9"/>
       <c r="B10" s="4" t="s">
         <v>15</v>
       </c>
@@ -700,7 +680,7 @@
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" ht="131.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="9" t="s">
         <v>36</v>
       </c>
       <c r="B11" s="5" t="s">

</xml_diff>

<commit_message>
Update Homework Assignments/a15/User Story Specs.xlsx
</commit_message>
<xml_diff>
--- a/Homework Assignments/a15/User Story Specs.xlsx
+++ b/Homework Assignments/a15/User Story Specs.xlsx
@@ -160,7 +160,7 @@
     <t>A graphical image that moves to show that the user won or not.</t>
   </si>
   <si>
-    <t>I, Eric, am a Twitch user HotdogWaterSnowcone, who wants to play around with the twitch commands. I type “!showHugs” into the chat box</t>
+    <t>I, Eric, am a Twitch user, HotdogWaterSnowcone, who wants to play around with the twitch commands. I type “!showHugs” into the chat box</t>
   </si>
   <si>
     <t xml:space="preserve">The !showHugs command triggers the intended functionality within the code       </t>
@@ -187,7 +187,7 @@
     <t>Show the user’s total amount of coins or points</t>
   </si>
   <si>
-    <t>I, Eric, am a Twitch user BigMusclesKevin, who wants to play around with the twitch commands. I type “!discipline” into the chat box</t>
+    <t>I, Eric, am a Twitch user, BigMusclesKevin, who wants to play around with the twitch commands. I type “!discipline” into the chat box</t>
   </si>
   <si>
     <t>Bot deducts one hug from the user and adds 1 count of discipline</t>

</xml_diff>